<commit_message>
Update: Fix import excel
</commit_message>
<xml_diff>
--- a/public/Template.xlsx
+++ b/public/Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Naufal Ammar H\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F75EDA0-D6A6-4FBB-A782-17FEAE450C0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA956727-82BF-4AB6-A0BE-11AE700569C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="14914" xr2:uid="{C3BC6170-B98B-4206-89CA-6E150A74B46C}"/>
   </bookViews>
@@ -25,23 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>Kode Asset Lama</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Lokasi</t>
   </si>
   <si>
-    <t>Kategori</t>
-  </si>
-  <si>
-    <t>Asset Position</t>
-  </si>
-  <si>
-    <t>Jenis</t>
-  </si>
-  <si>
     <t>Deskripsi</t>
   </si>
   <si>
@@ -51,9 +39,6 @@
     <t>Tanggal Perolehan</t>
   </si>
   <si>
-    <t>Umur Ekonomis (Tahun)</t>
-  </si>
-  <si>
     <t>Nilai Perolehan</t>
   </si>
   <si>
@@ -64,6 +49,30 @@
   </si>
   <si>
     <t>Dept</t>
+  </si>
+  <si>
+    <t>Kode Asset</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Specification</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>Installed Apps</t>
+  </si>
+  <si>
+    <t>Hand Over Date</t>
+  </si>
+  <si>
+    <t>NIK</t>
+  </si>
+  <si>
+    <t>Job Position</t>
   </si>
 </sst>
 </file>
@@ -462,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7210F671-66B7-488E-9E23-21BC8C84AFDD}">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:P1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -473,56 +482,63 @@
     <col min="1" max="1" width="19.07421875" style="3" customWidth="1"/>
     <col min="2" max="2" width="14.4609375" style="3" customWidth="1"/>
     <col min="3" max="3" width="15.23046875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="12.69140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.69140625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="18.07421875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="16.84375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="20.53515625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="20.3046875" style="4" customWidth="1"/>
-    <col min="10" max="10" width="21.84375" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="21.84375" style="3" customWidth="1"/>
-    <col min="13" max="13" width="17.765625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="12.69140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="18.07421875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="16.84375" style="3" customWidth="1"/>
+    <col min="7" max="9" width="20.53515625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="20.3046875" style="4" customWidth="1"/>
+    <col min="11" max="15" width="21.84375" style="3" customWidth="1"/>
+    <col min="16" max="16" width="17.765625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="O1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update: Fix data import
</commit_message>
<xml_diff>
--- a/public/Template.xlsx
+++ b/public/Template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Naufal Ammar H\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\MLP\ITAM\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA956727-82BF-4AB6-A0BE-11AE700569C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6D55AE7-832D-4DA0-A57F-BCDCB9C47A50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="14914" xr2:uid="{C3BC6170-B98B-4206-89CA-6E150A74B46C}"/>
   </bookViews>
@@ -30,9 +30,6 @@
     <t>Lokasi</t>
   </si>
   <si>
-    <t>Deskripsi</t>
-  </si>
-  <si>
     <t>Serial Number</t>
   </si>
   <si>
@@ -73,6 +70,9 @@
   </si>
   <si>
     <t>Job Position</t>
+  </si>
+  <si>
+    <t>Kategori</t>
   </si>
 </sst>
 </file>
@@ -474,7 +474,7 @@
   <dimension ref="A1:P1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -493,52 +493,52 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>